<commit_message>
Added AUDPC analysis for Frontiers submission
</commit_message>
<xml_diff>
--- a/data/AUDPC_HD.xlsx
+++ b/data/AUDPC_HD.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PhD document_3_7_19\Thesis Chapters\Chapter 7\QTL_analysis_desktop\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffitheduau-my.sharepoint.com/personal/i_bar_griffith_edu_au/Documents/Research/Supervision/Hari/QTL_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{583DE0B0-A1B7-436F-8802-055329F3AFDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{583DE0B0-A1B7-436F-8802-055329F3AFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B59CDFD0-CF90-47D7-80E5-50C79DECB3E4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{1ECAD14E-7A5D-4FF1-99F3-68053D891D88}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" activeTab="1" xr2:uid="{1ECAD14E-7A5D-4FF1-99F3-68053D891D88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="audpc_sqrt" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,8 +33,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={2CD6461C-1E21-46C8-A8E5-6E8696DA0370}</author>
+  </authors>
+  <commentList>
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{2CD6461C-1E21-46C8-A8E5-6E8696DA0370}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    These have been swapped to match prior data</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="145">
   <si>
     <t>RIL</t>
   </si>
@@ -41,12 +60,6 @@
     <t>Overall AUDPC SQ RT</t>
   </si>
   <si>
-    <t>ILWL 180</t>
-  </si>
-  <si>
-    <t>ILL 6002</t>
-  </si>
-  <si>
     <t>Sample_ID</t>
   </si>
   <si>
@@ -467,7 +480,13 @@
     <t>LOAL_143</t>
   </si>
   <si>
-    <t>Parent</t>
+    <t>ILW_180</t>
+  </si>
+  <si>
+    <t>ILL6002</t>
+  </si>
+  <si>
+    <t>Overall AUDPC SQRT</t>
   </si>
 </sst>
 </file>
@@ -501,12 +520,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -522,7 +547,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -535,12 +560,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="chemes]_x000d__x000a_Sci-Fi=_x000d__x000a_Nature=_x000d__x000a_robin=_x000d__x000a__x000d__x000a_[SoundScheme.Nature]_x000d__x000a_SystemAsterisk=C:\SNDSYS" xfId="1" xr:uid="{BAB76513-6B84-4BCB-8CBD-8808CDF772B7}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -562,6 +601,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Ido Bar" id="{025CECA4-E32B-41C0-B1AD-67255A43A017}" userId="Ido Bar" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -859,1577 +904,1585 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B39" dT="2021-06-30T03:53:52.13" personId="{025CECA4-E32B-41C0-B1AD-67255A43A017}" id="{2CD6461C-1E21-46C8-A8E5-6E8696DA0370}">
+    <text>These have been swapped to match prior data</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254DE94E-D28D-4A7A-B1C2-E403059FA59A}">
   <dimension ref="A1:C142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="3">
+        <v>180</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C2" s="4">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="3">
+        <v>6002</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="4">
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" s="4">
         <v>46.337538405872024</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="4">
         <v>38.610030472089178</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="4">
         <v>83.340020043073437</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="4">
         <v>113.30408612388365</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="4">
         <v>56.472923871224907</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="4">
         <v>124.92784888261066</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="5">
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" s="4">
         <v>95.753427828972903</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11" s="4">
         <v>98.146831040026882</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="5">
         <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12" s="4">
         <v>99.534121360276885</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="5">
         <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" s="4">
         <v>42.252635118713059</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="5">
         <v>23</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="4">
         <v>169.34875533567998</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="5">
         <v>25</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" s="4">
         <v>79.546460140482509</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="5">
         <v>26</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C16" s="4">
         <v>45.159590373939437</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="5">
         <v>28</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" s="4">
         <v>106.62019707323905</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="5">
         <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" s="4">
         <v>72.932156543854916</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="5">
         <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" s="4">
         <v>117.29088128229904</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="5">
         <v>31</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" s="4">
         <v>98.788404108342277</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="5">
         <v>32</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C21" s="4">
         <v>80.532801977386455</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="5">
         <v>33</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22" s="4">
         <v>51.40640457234062</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="5">
         <v>34</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C23" s="4">
         <v>61.973584777195427</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="5">
         <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C24" s="4">
         <v>96.925178516117199</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="5">
         <v>37</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C25" s="4">
         <v>54.860253093989442</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="5">
         <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C26" s="4">
         <v>67.783425281344449</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="5">
         <v>40</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C27" s="4">
         <v>94.137723911985788</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="5">
         <v>43</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C28" s="4">
         <v>92.144195982661415</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="5">
         <v>44</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C29" s="4">
         <v>157.13071837648363</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="5">
         <v>45</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C30" s="4">
         <v>55.275373506568563</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="5">
         <v>47</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C31" s="4">
         <v>130.03614108788838</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="5">
         <v>48</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C32" s="4">
         <v>64.652459979242565</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="5">
         <v>54</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C33" s="4">
         <v>46.524968625044238</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="5">
         <v>55</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C34" s="4">
         <v>118.5983555036789</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="5">
         <v>57</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C35" s="4">
         <v>63.293411903143422</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="5">
         <v>58</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C36" s="4">
         <v>71.949076315062626</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="5">
         <v>60</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C37" s="4">
         <v>24.989944717820443</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="5">
         <v>61</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C38" s="4">
         <v>47.644862580441924</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" s="6">
         <v>62</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>40</v>
+      <c r="B39" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="C39" s="4">
         <v>109.21019483234218</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" s="6">
         <v>63</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>41</v>
+      <c r="B40" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="C40" s="4">
         <v>60.049187956977548</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" s="5">
         <v>64</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C41" s="4">
         <v>78.392315030968916</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="5">
         <v>65</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C42" s="4">
         <v>15.652475842498529</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="5">
         <v>66</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C43" s="4">
         <v>27.215007424363947</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="5">
         <v>67</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C44" s="4">
         <v>89.710593105637997</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="5">
         <v>68</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C45" s="4">
         <v>124.95849736003773</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" s="5">
         <v>69</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C46" s="4">
         <v>88.27083780042193</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" s="5">
         <v>70</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C47" s="4">
         <v>130.5320617542011</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" s="5">
         <v>73</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C48" s="4">
         <v>22.159493977308426</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="5">
         <v>74</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C49" s="4">
         <v>36.8932393686311</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" s="5">
         <v>75</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C50" s="4">
         <v>72.956629037585287</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" s="5">
         <v>77</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C51" s="4">
         <v>30.329280713535528</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" s="5">
         <v>79</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C52" s="4">
         <v>79.337708481739611</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53" s="5">
         <v>81</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C53" s="4">
         <v>63.195683700340609</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" s="5">
         <v>82</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C54" s="4">
         <v>11.992293532375975</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" s="5">
         <v>83</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C55" s="4">
         <v>96.68925604216281</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" s="5">
         <v>84</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C56" s="4">
         <v>38.188130791298661</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" s="5">
         <v>85</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C57" s="4">
         <v>99.036807903303881</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" s="5">
         <v>86</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C58" s="4">
         <v>10.34995223910953</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59" s="5">
         <v>87</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C59" s="4">
         <v>59.633962506724274</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60" s="5">
         <v>88</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C60" s="4">
         <v>110.62783263728971</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61" s="5">
         <v>89</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C61" s="4">
         <v>48.307168630682483</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62" s="5">
         <v>90</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C62" s="4">
         <v>71.914540894545496</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63" s="5">
         <v>91</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C63" s="4">
         <v>150.03291337208719</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" s="5">
         <v>92</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C64" s="4">
         <v>51.122064012227511</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65" s="5">
         <v>94</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C65" s="4">
         <v>87.044562579428288</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66" s="5">
         <v>96</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C66" s="4">
         <v>54.019199538070282</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67" s="5">
         <v>99</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C67" s="4">
         <v>44.088051082057291</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A68" s="5">
         <v>100</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C68" s="4">
         <v>108.40403437614245</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A69" s="5">
         <v>101</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C69" s="4">
         <v>111.9276757457808</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A70" s="5">
         <v>103</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C70" s="4">
         <v>75.779834903991215</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71" s="5">
         <v>104</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C71" s="4">
         <v>121.80791422117449</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72" s="5">
         <v>105</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C72" s="4">
         <v>113.97555207781065</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A73" s="5">
         <v>106</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C73" s="4">
         <v>72.440815966621443</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A74" s="5">
         <v>108</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C74" s="4">
         <v>111.79654947815219</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A75" s="5">
         <v>109</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C75" s="4">
         <v>24.748737341529164</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A76" s="5">
         <v>110</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C76" s="4">
         <v>50.995125453947352</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A77" s="5">
         <v>111</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C77" s="4">
         <v>101.31798473809042</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A78" s="5">
         <v>112</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C78" s="4">
         <v>28.352375730254622</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A79" s="5">
         <v>114</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C79" s="4">
         <v>13.363062095621219</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A80" s="5">
         <v>116</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C80" s="4">
         <v>6.6815310478106094</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A81" s="5">
         <v>117</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C81" s="4">
         <v>116.16079520373403</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82" s="5">
         <v>118</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C82" s="4">
         <v>58.011935111532132</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83" s="5">
         <v>119</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C83" s="4">
         <v>30.40991237944138</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" s="5">
         <v>120</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C84" s="4">
         <v>75.643080397150783</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85" s="5">
         <v>121</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C85" s="4">
         <v>67.749071794630083</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A86" s="5">
         <v>122</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C86" s="4">
         <v>54.829089837452045</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A87" s="5">
         <v>123</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C87" s="4">
         <v>3.2274861218395143</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A88" s="5">
         <v>124</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C88" s="4">
         <v>48.958907795934174</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A89" s="5">
         <v>125</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C89" s="4">
         <v>79.12168155773486</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A90" s="5">
         <v>126</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C90" s="4">
         <v>79.005379433988537</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A91" s="5">
         <v>127</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C91" s="4">
         <v>36.69743187283224</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A92" s="5">
         <v>129</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C92" s="4">
         <v>41.803183977515388</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A93" s="5">
         <v>130</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C93" s="4">
         <v>71.848370662245301</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A94" s="5">
         <v>132</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C94" s="4">
         <v>139.90923061716541</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A95" s="5">
         <v>133</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C95" s="4">
         <v>74.126548870157734</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A96" s="5">
         <v>134</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C96" s="4">
         <v>87.011590070553794</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A97" s="5">
         <v>136</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C97" s="4">
         <v>108.23774554374236</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A98" s="5">
         <v>137</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C98" s="4">
         <v>103.26777896696427</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A99" s="5">
         <v>138</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C99" s="4">
         <v>106.82449007473144</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A100" s="5">
         <v>139</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C100" s="4">
         <v>74.869571811772062</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A101" s="5">
         <v>140</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C101" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A102" s="5">
         <v>141</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C102" s="4">
         <v>51.153873056392115</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A103" s="5">
         <v>142</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C103" s="4">
         <v>86.081249835828544</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A104" s="5">
         <v>143</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C104" s="4">
         <v>37.857732008541348</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A105" s="5">
         <v>145</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C105" s="4">
         <v>40.796607195443265</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A106" s="5">
         <v>146</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C106" s="4">
         <v>166.53868361486278</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A107" s="5">
         <v>147</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C107" s="4">
         <v>32.179064455504417</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A108" s="5">
         <v>148</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C108" s="4">
         <v>120.60739201550223</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A109" s="5">
         <v>149</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C109" s="4">
         <v>134.36123893256263</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A110" s="5">
         <v>152</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C110" s="4">
         <v>87.263513268042232</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A111" s="5">
         <v>154</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C111" s="4">
         <v>42.446590109535862</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A112" s="5">
         <v>155</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C112" s="4">
         <v>139.98770873105065</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A113" s="5">
         <v>157</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C113" s="4">
         <v>53.080144287647542</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A114" s="5">
         <v>158</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C114" s="4">
         <v>57.383714870633156</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A115" s="5">
         <v>160</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C115" s="4">
         <v>133.35418519850555</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A116" s="5">
         <v>162</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C116" s="4">
         <v>84.304636067252133</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A117" s="5">
         <v>163</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C117" s="4">
         <v>33.159080343990887</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A118" s="5">
         <v>164</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C118" s="4">
         <v>14.293440963681721</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A119" s="5">
         <v>167</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C119" s="4">
         <v>97.538979755809407</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A120" s="5">
         <v>168</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C120" s="4">
         <v>46.224873734152915</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A121" s="5">
         <v>169</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C121" s="4">
         <v>61.096379428290859</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A122" s="5">
         <v>170</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C122" s="4">
         <v>78.910310361172506</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A123" s="5">
         <v>171</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C123" s="4">
         <v>11.796383174709248</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A124" s="5">
         <v>172</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C124" s="4">
         <v>104.92012068393947</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A125" s="5">
         <v>175</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C125" s="4">
         <v>77.127411509492688</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A126" s="5">
         <v>179</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C126" s="4">
         <v>43.020032027090217</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A127" s="5">
         <v>181</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C127" s="4">
         <v>139.60694826541061</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A128" s="5">
         <v>182</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C128" s="4">
         <v>73.035599694807232</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A129" s="5">
         <v>183</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C129" s="4">
         <v>78.875237408723848</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A130" s="5">
         <v>184</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C130" s="4">
         <v>72.6004991966836</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A131" s="5">
         <v>185</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C131" s="4">
         <v>55.960028219550736</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A132" s="5">
         <v>186</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C132" s="4">
         <v>59.601930026170322</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A133" s="5">
         <v>188</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C133" s="4">
         <v>78.559500771767134</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A134" s="5">
         <v>189</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C134" s="4">
         <v>56.082864782822142</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A135" s="5">
         <v>190</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C135" s="4">
         <v>108.86886546179011</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A136" s="5">
         <v>192</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C136" s="4">
         <v>77.860118106343464</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A137" s="5">
         <v>193</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C137" s="4">
         <v>54.401351428098351</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A138" s="5">
         <v>194</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C138" s="4">
         <v>127.80193008453874</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A139" s="5">
         <v>195</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C139" s="4">
         <v>128.7107702920477</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A140" s="5">
         <v>196</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C140" s="4">
         <v>29.320561368532186</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A141" s="5">
         <v>197</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C141" s="4">
         <v>85.404431090647677</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A142" s="5">
         <v>198</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C142" s="4">
         <v>148.31272048007548</v>
@@ -2437,9 +2490,1595 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:B142">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D59115B-3029-46B1-934E-FCA7196D4C32}">
+  <dimension ref="A1:C142"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="3">
+        <v>180</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="3">
+        <v>6002</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="4">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4">
+        <v>46.337538405872024</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
+        <v>38.610030472089178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4">
+        <v>83.340020043073437</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="5">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4">
+        <v>113.30408612388365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="5">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4">
+        <v>56.472923871224907</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="5">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4">
+        <v>124.92784888261066</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="5">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4">
+        <v>95.753427828972903</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="5">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4">
+        <v>98.146831040026882</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="5">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4">
+        <v>99.534121360276885</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="5">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4">
+        <v>42.252635118713059</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="5">
+        <v>23</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4">
+        <v>169.34875533567998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="5">
+        <v>25</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="4">
+        <v>79.546460140482509</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="5">
+        <v>26</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4">
+        <v>45.159590373939437</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="5">
+        <v>28</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="4">
+        <v>106.62019707323905</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="5">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="4">
+        <v>72.932156543854916</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="5">
+        <v>30</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="4">
+        <v>117.29088128229904</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="5">
+        <v>31</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="4">
+        <v>98.788404108342277</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="5">
+        <v>32</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="4">
+        <v>80.532801977386455</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="5">
+        <v>33</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="4">
+        <v>51.40640457234062</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="5">
+        <v>34</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="4">
+        <v>61.973584777195427</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="5">
+        <v>36</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="4">
+        <v>96.925178516117199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" s="5">
+        <v>37</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="4">
+        <v>54.860253093989442</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" s="5">
+        <v>38</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="4">
+        <v>67.783425281344449</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" s="5">
+        <v>40</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="4">
+        <v>94.137723911985788</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" s="5">
+        <v>43</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="4">
+        <v>92.144195982661415</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" s="5">
+        <v>44</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="4">
+        <v>157.13071837648363</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" s="5">
+        <v>45</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="4">
+        <v>55.275373506568563</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" s="5">
+        <v>47</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="4">
+        <v>130.03614108788838</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" s="5">
+        <v>48</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="4">
+        <v>64.652459979242565</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" s="5">
+        <v>54</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="4">
+        <v>46.524968625044238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" s="5">
+        <v>55</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="4">
+        <v>118.5983555036789</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" s="5">
+        <v>57</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="4">
+        <v>63.293411903143422</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" s="5">
+        <v>58</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="4">
+        <v>71.949076315062626</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" s="5">
+        <v>60</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="4">
+        <v>24.989944717820443</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" s="5">
+        <v>61</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="4">
+        <v>47.644862580441924</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" s="6">
+        <v>62</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="4">
+        <v>109.21019483234218</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" s="6">
+        <v>63</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="4">
+        <v>60.049187956977548</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" s="5">
+        <v>64</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="4">
+        <v>78.392315030968916</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" s="5">
+        <v>65</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="4">
+        <v>15.652475842498529</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" s="5">
+        <v>66</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="4">
+        <v>27.215007424363947</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A44" s="5">
+        <v>67</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="4">
+        <v>89.710593105637997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45" s="5">
+        <v>68</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="4">
+        <v>124.95849736003773</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A46" s="5">
+        <v>69</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="4">
+        <v>88.27083780042193</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A47" s="5">
+        <v>70</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" s="4">
+        <v>130.5320617542011</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A48" s="5">
+        <v>73</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" s="4">
+        <v>22.159493977308426</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49" s="5">
+        <v>74</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="4">
+        <v>36.8932393686311</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A50" s="5">
+        <v>75</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" s="4">
+        <v>72.956629037585287</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51" s="5">
+        <v>77</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" s="4">
+        <v>30.329280713535528</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A52" s="5">
+        <v>79</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" s="4">
+        <v>79.337708481739611</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A53" s="5">
+        <v>81</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" s="4">
+        <v>63.195683700340609</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A54" s="5">
+        <v>82</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="4">
+        <v>11.992293532375975</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A55" s="5">
+        <v>83</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" s="4">
+        <v>96.68925604216281</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A56" s="5">
+        <v>84</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="4">
+        <v>38.188130791298661</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A57" s="5">
+        <v>85</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" s="4">
+        <v>99.036807903303881</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A58" s="5">
+        <v>86</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C58" s="4">
+        <v>10.34995223910953</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A59" s="5">
+        <v>87</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C59" s="4">
+        <v>59.633962506724274</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A60" s="5">
+        <v>88</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60" s="4">
+        <v>110.62783263728971</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A61" s="5">
+        <v>89</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C61" s="4">
+        <v>48.307168630682483</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A62" s="5">
+        <v>90</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C62" s="4">
+        <v>71.914540894545496</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A63" s="5">
+        <v>91</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C63" s="4">
+        <v>150.03291337208719</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A64" s="5">
+        <v>92</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C64" s="4">
+        <v>51.122064012227511</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A65" s="5">
+        <v>94</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C65" s="4">
+        <v>87.044562579428288</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A66" s="5">
+        <v>96</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C66" s="4">
+        <v>54.019199538070282</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A67" s="5">
+        <v>99</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C67" s="4">
+        <v>44.088051082057291</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A68" s="5">
+        <v>100</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C68" s="4">
+        <v>108.40403437614245</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A69" s="5">
+        <v>101</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C69" s="4">
+        <v>111.9276757457808</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A70" s="5">
+        <v>103</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C70" s="4">
+        <v>75.779834903991215</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A71" s="5">
+        <v>104</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C71" s="4">
+        <v>121.80791422117449</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A72" s="5">
+        <v>105</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C72" s="4">
+        <v>113.97555207781065</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A73" s="5">
+        <v>106</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C73" s="4">
+        <v>72.440815966621443</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A74" s="5">
+        <v>108</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C74" s="4">
+        <v>111.79654947815219</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A75" s="5">
+        <v>109</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C75" s="4">
+        <v>24.748737341529164</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A76" s="5">
+        <v>110</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C76" s="4">
+        <v>50.995125453947352</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A77" s="5">
+        <v>111</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C77" s="4">
+        <v>101.31798473809042</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A78" s="5">
+        <v>112</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C78" s="4">
+        <v>28.352375730254622</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A79" s="5">
+        <v>114</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C79" s="4">
+        <v>13.363062095621219</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A80" s="5">
+        <v>116</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C80" s="4">
+        <v>6.6815310478106094</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A81" s="5">
+        <v>117</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C81" s="4">
+        <v>116.16079520373403</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A82" s="5">
+        <v>118</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C82" s="4">
+        <v>58.011935111532132</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A83" s="5">
+        <v>119</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C83" s="4">
+        <v>30.40991237944138</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A84" s="5">
+        <v>120</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C84" s="4">
+        <v>75.643080397150783</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A85" s="5">
+        <v>121</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C85" s="4">
+        <v>67.749071794630083</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A86" s="5">
+        <v>122</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C86" s="4">
+        <v>54.829089837452045</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A87" s="5">
+        <v>123</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C87" s="4">
+        <v>3.2274861218395143</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A88" s="5">
+        <v>124</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C88" s="4">
+        <v>48.958907795934174</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A89" s="5">
+        <v>125</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C89" s="4">
+        <v>79.12168155773486</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A90" s="5">
+        <v>126</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C90" s="4">
+        <v>79.005379433988537</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A91" s="5">
+        <v>127</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C91" s="4">
+        <v>36.69743187283224</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A92" s="5">
+        <v>129</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C92" s="4">
+        <v>41.803183977515388</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A93" s="5">
+        <v>130</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C93" s="4">
+        <v>71.848370662245301</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A94" s="5">
+        <v>132</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C94" s="4">
+        <v>139.90923061716541</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A95" s="5">
+        <v>133</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C95" s="4">
+        <v>74.126548870157734</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A96" s="5">
+        <v>134</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C96" s="4">
+        <v>87.011590070553794</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A97" s="5">
+        <v>136</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C97" s="4">
+        <v>108.23774554374236</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A98" s="5">
+        <v>137</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C98" s="4">
+        <v>103.26777896696427</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A99" s="5">
+        <v>138</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C99" s="4">
+        <v>106.82449007473144</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A100" s="5">
+        <v>139</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C100" s="4">
+        <v>74.869571811772062</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A101" s="5">
+        <v>140</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C101" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A102" s="5">
+        <v>141</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C102" s="4">
+        <v>51.153873056392115</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A103" s="5">
+        <v>142</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C103" s="4">
+        <v>86.081249835828544</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A104" s="5">
+        <v>143</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C104" s="4">
+        <v>37.857732008541348</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A105" s="5">
+        <v>145</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C105" s="4">
+        <v>40.796607195443265</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A106" s="5">
+        <v>146</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C106" s="4">
+        <v>166.53868361486278</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A107" s="5">
+        <v>147</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C107" s="4">
+        <v>32.179064455504417</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A108" s="5">
+        <v>148</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C108" s="4">
+        <v>120.60739201550223</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A109" s="5">
+        <v>149</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C109" s="4">
+        <v>134.36123893256263</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A110" s="5">
+        <v>152</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C110" s="4">
+        <v>87.263513268042232</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A111" s="5">
+        <v>154</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C111" s="4">
+        <v>42.446590109535862</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A112" s="5">
+        <v>155</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C112" s="4">
+        <v>139.98770873105065</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A113" s="5">
+        <v>157</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C113" s="4">
+        <v>53.080144287647542</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A114" s="5">
+        <v>158</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C114" s="4">
+        <v>57.383714870633156</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A115" s="5">
+        <v>160</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C115" s="4">
+        <v>133.35418519850555</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A116" s="5">
+        <v>162</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C116" s="4">
+        <v>84.304636067252133</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A117" s="5">
+        <v>163</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C117" s="4">
+        <v>33.159080343990887</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A118" s="5">
+        <v>164</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C118" s="4">
+        <v>14.293440963681721</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A119" s="5">
+        <v>167</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C119" s="4">
+        <v>97.538979755809407</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A120" s="5">
+        <v>168</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C120" s="4">
+        <v>46.224873734152915</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A121" s="5">
+        <v>169</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C121" s="4">
+        <v>61.096379428290859</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A122" s="5">
+        <v>170</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C122" s="4">
+        <v>78.910310361172506</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A123" s="5">
+        <v>171</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C123" s="4">
+        <v>11.796383174709248</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A124" s="5">
+        <v>172</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C124" s="4">
+        <v>104.92012068393947</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A125" s="5">
+        <v>175</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C125" s="4">
+        <v>77.127411509492688</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A126" s="5">
+        <v>179</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C126" s="4">
+        <v>43.020032027090217</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A127" s="5">
+        <v>181</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C127" s="4">
+        <v>139.60694826541061</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A128" s="5">
+        <v>182</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C128" s="4">
+        <v>73.035599694807232</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A129" s="5">
+        <v>183</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C129" s="4">
+        <v>78.875237408723848</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A130" s="5">
+        <v>184</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C130" s="4">
+        <v>72.6004991966836</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A131" s="5">
+        <v>185</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C131" s="4">
+        <v>55.960028219550736</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A132" s="5">
+        <v>186</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C132" s="4">
+        <v>59.601930026170322</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A133" s="5">
+        <v>188</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C133" s="4">
+        <v>78.559500771767134</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A134" s="5">
+        <v>189</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C134" s="4">
+        <v>56.082864782822142</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A135" s="5">
+        <v>190</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C135" s="4">
+        <v>108.86886546179011</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A136" s="5">
+        <v>192</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C136" s="4">
+        <v>77.860118106343464</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A137" s="5">
+        <v>193</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C137" s="4">
+        <v>54.401351428098351</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A138" s="5">
+        <v>194</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C138" s="4">
+        <v>127.80193008453874</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A139" s="5">
+        <v>195</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C139" s="4">
+        <v>128.7107702920477</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A140" s="5">
+        <v>196</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C140" s="4">
+        <v>29.320561368532186</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A141" s="5">
+        <v>197</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C141" s="4">
+        <v>85.404431090647677</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A142" s="5">
+        <v>198</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C142" s="4">
+        <v>148.31272048007548</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B4:B142">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>